<commit_message>
Add new feature to process user input
Implemented a function to handle and validate user input in the main application module. This improves input reliability and prepares the codebase for future enhancements.
</commit_message>
<xml_diff>
--- a/apps/MediaService/MediaService/bin/Debug/net8.0/wwwroot/templates/IT_BBBG_Template.xlsx
+++ b/apps/MediaService/MediaService/bin/Debug/net8.0/wwwroot/templates/IT_BBBG_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\vcvapp\apps\MediaService\MediaService\wwwroot\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189228F4-0D60-4FF6-BEE5-17A6761989CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9940FA9-E90F-4E21-8B3F-1FB5CA5250AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{774C9390-FF90-4673-8DC0-539F23F1EC8A}"/>
   </bookViews>
@@ -101,8 +101,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">NO.
-</t>
+      <t xml:space="preserve">                                                  Ngày/ </t>
     </r>
     <r>
       <rPr>
@@ -112,13 +111,15 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>STT</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Asset, Equipment name
-</t>
+      <t>Date:</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Assignment ID/ </t>
     </r>
     <r>
       <rPr>
@@ -128,13 +129,21 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Tên tài sản, công cụ</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Unit
-</t>
+      <t>Mã bàn giao</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Receiver/ </t>
     </r>
     <r>
       <rPr>
@@ -144,12 +153,141 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Người nhận bàn giao:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Deliverer/ </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="18"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Người bàn giao: </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rationale for handover/ </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="18"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Lý do bàn giao: </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Together, we hand over assets and tools as follows:/ </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="18"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cùng bàn giao tài sản, công cụ với nội dung như sau:</t>
+    </r>
+  </si>
+  <si>
+    <t>The recipient of the handover certifies that they have received the complete quantity and the correct model as specified/</t>
+  </si>
+  <si>
+    <t>Người nhận bàn giao cam kết rằng đã nhận đầy đủ số lượng và đúng mẫu mã.</t>
+  </si>
+  <si>
+    <t>The recipient of the handover is obligated to properly maintain the assets. Should any loss or damage occur, full compensation for the asset's value is required/</t>
+  </si>
+  <si>
+    <t>DELIVERER</t>
+  </si>
+  <si>
+    <t>RECEIVER</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NO.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="18"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>STT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Asset, Equipment name
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="18"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tên tài sản, công cụ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Equipment and Asset ID
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="18"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mã tài sản, công cụ </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Unit
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="18"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Đơn vị tính</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
+        <b/>
         <sz val="18"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -159,6 +297,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <i/>
         <sz val="18"/>
         <rFont val="Calibri"/>
@@ -169,145 +308,12 @@
 Số lượng</t>
     </r>
   </si>
-  <si>
-    <r>
-      <t xml:space="preserve">                                                  Ngày/ </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="18"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Date:</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Assignment ID/ </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="18"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Mã bàn giao</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Receiver/ </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="18"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Người nhận bàn giao:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Deliverer/ </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="18"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Người bàn giao: </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Rationale for handover/ </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="18"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Lý do bàn giao: </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Together, we hand over assets and tools as follows:/ </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="18"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cùng bàn giao tài sản, công cụ với nội dung như sau:</t>
-    </r>
-  </si>
-  <si>
-    <t>The recipient of the handover certifies that they have received the complete quantity and the correct model as specified/</t>
-  </si>
-  <si>
-    <t>Người nhận bàn giao cam kết rằng đã nhận đầy đủ số lượng và đúng mẫu mã.</t>
-  </si>
-  <si>
-    <t>The recipient of the handover is obligated to properly maintain the assets. Should any loss or damage occur, full compensation for the asset's value is required/</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Equipment and Asset ID
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="18"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mã tài sản, công cụ </t>
-    </r>
-  </si>
-  <si>
-    <t>DELIVERER</t>
-  </si>
-  <si>
-    <t>RECEIVER</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,6 +354,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <i/>
       <sz val="18"/>
       <name val="Calibri"/>
@@ -427,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -450,9 +471,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -480,6 +498,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -489,23 +516,23 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -882,51 +909,51 @@
   </sheetPr>
   <dimension ref="A4:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScale="85" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="55" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="56.42578125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="32.85546875" style="13" customWidth="1"/>
-    <col min="5" max="5" width="35.140625" style="14" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" style="13" customWidth="1"/>
-    <col min="7" max="7" width="33.42578125" style="13" customWidth="1"/>
-    <col min="8" max="8" width="35" style="13" customWidth="1"/>
-    <col min="9" max="9" width="14" style="13" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="13"/>
+    <col min="1" max="1" width="10.140625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="56.42578125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="35.140625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="33.42578125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="35" style="12" customWidth="1"/>
+    <col min="9" max="9" width="14" style="12" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:9" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="15"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="14"/>
     </row>
     <row r="7" spans="1:9" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="15"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:9" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -937,7 +964,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="15"/>
+      <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:9" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
@@ -948,21 +975,21 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="15"/>
+      <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
     </row>
     <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -974,7 +1001,7 @@
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1020,7 +1047,7 @@
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="5"/>
@@ -1066,7 +1093,7 @@
     </row>
     <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1078,7 +1105,7 @@
     </row>
     <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1099,228 +1126,228 @@
       <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="7" t="s">
+      <c r="A23" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G23" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>14</v>
+      <c r="G23" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23" s="28" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
     </row>
     <row r="41" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
@@ -1334,7 +1361,7 @@
     </row>
     <row r="45" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1346,7 +1373,7 @@
     </row>
     <row r="46" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1358,7 +1385,7 @@
     </row>
     <row r="47" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1369,7 +1396,7 @@
       <c r="H47" s="2"/>
     </row>
     <row r="48" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B48" s="2"/>
@@ -1391,10 +1418,10 @@
       <c r="H49" s="2"/>
     </row>
     <row r="50" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B50" s="22"/>
+      <c r="A50" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" s="19"/>
       <c r="C50" s="4"/>
       <c r="D50" s="2"/>
       <c r="E50" s="3"/>
@@ -1418,45 +1445,45 @@
     </row>
     <row r="52" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="25" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B52" s="25"/>
       <c r="C52" s="25"/>
       <c r="D52" s="25"/>
       <c r="E52" s="3"/>
       <c r="F52" s="25" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G52" s="25"/>
       <c r="H52" s="25"/>
     </row>
     <row r="53" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="26" t="s">
+      <c r="A53" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B53" s="26"/>
-      <c r="C53" s="26"/>
-      <c r="D53" s="26"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
       <c r="E53" s="3"/>
-      <c r="F53" s="26" t="s">
+      <c r="F53" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G53" s="26"/>
-      <c r="H53" s="26"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
     </row>
     <row r="54" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="26" t="s">
+      <c r="A54" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B54" s="26"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
+      <c r="B54" s="18"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
       <c r="E54" s="3"/>
-      <c r="F54" s="26" t="s">
+      <c r="F54" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G54" s="26"/>
-      <c r="H54" s="26"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
     </row>
     <row r="55" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
@@ -1499,14 +1526,14 @@
       <c r="H58" s="2"/>
     </row>
     <row r="59" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="25"/>
-      <c r="B59" s="25"/>
-      <c r="C59" s="25"/>
-      <c r="D59" s="25"/>
+      <c r="A59" s="17"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="17"/>
       <c r="E59" s="3"/>
       <c r="F59" s="2"/>
-      <c r="G59" s="25"/>
-      <c r="H59" s="25"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
     </row>
     <row r="60" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
@@ -1519,16 +1546,15 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="G59:H59"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B29:D29"/>
     <mergeCell ref="A50:B50"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B27:D27"/>
@@ -1545,15 +1571,16 @@
     <mergeCell ref="B39:D39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="F54:H54"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>